<commit_message>
Wei will work on the files from: 4 - 39
git-svn-id: https://subversion.ucar.edu/ncldev/ncarg/branches/NCL_6_0_0@11699 10fe2890-8a40-4696-8b1d-7ccbb19c398e
</commit_message>
<xml_diff>
--- a/ni/src/lib/nfp/NfpSrcList.xlsx
+++ b/ni/src/lib/nfp/NfpSrcList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="340" windowWidth="20220" windowHeight="27980" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="22260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,96 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="139">
+  <si>
+    <t>sg_toolsW.c</t>
+  </si>
+  <si>
+    <t>shgridW.c</t>
+  </si>
+  <si>
+    <t>simpsonW.c</t>
+  </si>
+  <si>
+    <t>sindexW.c</t>
+  </si>
+  <si>
+    <t>skewtW.c</t>
+  </si>
+  <si>
+    <t>slpW.c</t>
+  </si>
+  <si>
+    <t>smth9W.c</t>
+  </si>
+  <si>
+    <t>sortW.c</t>
+  </si>
+  <si>
+    <t>space_timeW.c</t>
+  </si>
+  <si>
+    <t>spanW.c</t>
+  </si>
+  <si>
+    <t>spcorrW.c</t>
+  </si>
+  <si>
+    <t>specxW.c</t>
+  </si>
+  <si>
+    <t>sph2W.c</t>
+  </si>
+  <si>
+    <t>sphintW.c</t>
+  </si>
+  <si>
+    <t>sstoiW.c</t>
+  </si>
+  <si>
+    <t>statW.c</t>
+  </si>
+  <si>
+    <t>stdatmusW.c</t>
+  </si>
+  <si>
+    <t>studentW.c</t>
+  </si>
+  <si>
+    <t>svdW.c</t>
+  </si>
+  <si>
+    <t>taperW.c</t>
+  </si>
+  <si>
+    <t>tdpackW.c</t>
+  </si>
+  <si>
+    <t>tempnamW.c</t>
+  </si>
+  <si>
+    <t>Wei</t>
+  </si>
+  <si>
+    <t>Wei</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wei</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wei</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wei</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wei</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>tropwmoW.c</t>
   </si>
@@ -406,77 +495,17 @@
   <si>
     <t>ripW.c</t>
   </si>
-  <si>
-    <t>sg_toolsW.c</t>
-  </si>
-  <si>
-    <t>shgridW.c</t>
-  </si>
-  <si>
-    <t>simpsonW.c</t>
-  </si>
-  <si>
-    <t>sindexW.c</t>
-  </si>
-  <si>
-    <t>skewtW.c</t>
-  </si>
-  <si>
-    <t>slpW.c</t>
-  </si>
-  <si>
-    <t>smth9W.c</t>
-  </si>
-  <si>
-    <t>sortW.c</t>
-  </si>
-  <si>
-    <t>space_timeW.c</t>
-  </si>
-  <si>
-    <t>spanW.c</t>
-  </si>
-  <si>
-    <t>spcorrW.c</t>
-  </si>
-  <si>
-    <t>specxW.c</t>
-  </si>
-  <si>
-    <t>sph2W.c</t>
-  </si>
-  <si>
-    <t>sphintW.c</t>
-  </si>
-  <si>
-    <t>sstoiW.c</t>
-  </si>
-  <si>
-    <t>statW.c</t>
-  </si>
-  <si>
-    <t>stdatmusW.c</t>
-  </si>
-  <si>
-    <t>studentW.c</t>
-  </si>
-  <si>
-    <t>svdW.c</t>
-  </si>
-  <si>
-    <t>taperW.c</t>
-  </si>
-  <si>
-    <t>tdpackW.c</t>
-  </si>
-  <si>
-    <t>tempnamW.c</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -544,12 +573,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:D257"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A75" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124:A125"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -892,659 +922,767 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>33</v>
+        <v>61</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>34</v>
+        <v>62</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>35</v>
+        <v>63</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>36</v>
+        <v>64</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>65</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>38</v>
+        <v>66</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>39</v>
+        <v>67</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>41</v>
+        <v>69</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>42</v>
+        <v>70</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>43</v>
+        <v>71</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>44</v>
+        <v>72</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>73</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>74</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
+        <v>75</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
+        <v>76</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
+        <v>77</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
+        <v>78</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
+        <v>79</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
+        <v>80</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
+        <v>81</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
+        <v>82</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
+        <v>83</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
+        <v>84</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
+        <v>85</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
+        <v>86</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
+        <v>87</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
+        <v>88</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
+        <v>89</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
+        <v>90</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
+        <v>91</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
+        <v>92</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
+        <v>93</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
+        <v>94</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
+        <v>95</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
+        <v>96</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="4" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="4" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="4" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="4" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="4" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="4" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="4" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="4" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="4" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="4" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="4" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="4" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="4" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="4" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="4" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="4" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="4" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="4" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="4" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="4" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="4" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="4" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="4" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="4" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="4" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="4" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="4" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="4" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="4" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="4" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="4" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="4" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="4" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="4" t="s">
-        <v>111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="4" t="s">
-        <v>112</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="4" t="s">
-        <v>113</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="4" t="s">
-        <v>114</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="4" t="s">
-        <v>115</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="4" t="s">
-        <v>116</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="4" t="s">
-        <v>117</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="4" t="s">
-        <v>118</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="4" t="s">
-        <v>119</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="4" t="s">
-        <v>120</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="4" t="s">
-        <v>121</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="4" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="4" t="s">
-        <v>123</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="4" t="s">
-        <v>124</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" s="4" t="s">
-        <v>125</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="4" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="4" t="s">
-        <v>127</v>
+        <v>16</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="4" t="s">
-        <v>128</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="4" t="s">
-        <v>129</v>
+        <v>18</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="4" t="s">
-        <v>130</v>
+        <v>19</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="4" t="s">
-        <v>131</v>
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="4" t="s">
-        <v>132</v>
+        <v>21</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="4" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="4" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" s="4" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="4" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" s="4" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="4" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="4" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="4" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" s="4" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="4" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="4" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="4" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="4" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="4" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="4" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="4" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="4" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="D125" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="4" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" s="4" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" s="4" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
     </row>
     <row r="131" spans="1:1">
@@ -1927,6 +2065,11 @@
     </row>
     <row r="257" spans="1:1">
       <c r="A257" s="4"/>
+    </row>
+    <row r="1048576" spans="3:3">
+      <c r="C1048576" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
reserve more files for Wei
git-svn-id: https://subversion.ucar.edu/ncldev/ncarg/branches/NCL_6_0_0@11710 10fe2890-8a40-4696-8b1d-7ccbb19c398e
</commit_message>
<xml_diff>
--- a/ni/src/lib/nfp/NfpSrcList.xlsx
+++ b/ni/src/lib/nfp/NfpSrcList.xlsx
@@ -19,7 +19,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="140">
+  <si>
+    <t>mapgciW.c</t>
+  </si>
+  <si>
+    <t>mixhumW.c</t>
+  </si>
+  <si>
+    <t>mocloopsW.c</t>
+  </si>
+  <si>
+    <t>natgridW.c</t>
+  </si>
+  <si>
+    <t>ncl2v5dW.c</t>
+  </si>
+  <si>
+    <t>ncolorW.c</t>
+  </si>
+  <si>
+    <t>nglogoW.c</t>
+  </si>
+  <si>
+    <t>ngmiscW.c</t>
+  </si>
+  <si>
+    <t>nicevalsW.c</t>
+  </si>
+  <si>
+    <t>objanalW.c</t>
+  </si>
+  <si>
+    <t>omcalc_ccmW.c</t>
+  </si>
+  <si>
+    <t>outputgif.c</t>
+  </si>
+  <si>
+    <t>paleoW.c</t>
+  </si>
+  <si>
+    <t>pdfW.c</t>
+  </si>
+  <si>
+    <t>poissonW.c</t>
+  </si>
+  <si>
+    <t>prcwatW.c</t>
+  </si>
+  <si>
+    <t>preshybW.c</t>
+  </si>
+  <si>
+    <t>pressigW.c</t>
+  </si>
+  <si>
+    <t>probtestW.c</t>
+  </si>
+  <si>
+    <t>randomW.c</t>
+  </si>
+  <si>
+    <t>rcmW.c</t>
+  </si>
+  <si>
+    <t>reduce2reg.f90</t>
+  </si>
+  <si>
+    <t>regcoefW.c</t>
+  </si>
+  <si>
+    <t>regridtst.f90</t>
+  </si>
+  <si>
+    <t>relhumW.c</t>
+  </si>
+  <si>
+    <t>remapW.c</t>
+  </si>
+  <si>
+    <t>rhombtriW.c</t>
+  </si>
+  <si>
+    <t>ripW.c</t>
+  </si>
   <si>
     <t>sg_toolsW.c</t>
   </si>
@@ -107,6 +191,10 @@
   </si>
   <si>
     <t>Wei</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Updated</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -410,90 +498,6 @@
   </si>
   <si>
     <t>lspolyW.c</t>
-  </si>
-  <si>
-    <t>mapgciW.c</t>
-  </si>
-  <si>
-    <t>mixhumW.c</t>
-  </si>
-  <si>
-    <t>mocloopsW.c</t>
-  </si>
-  <si>
-    <t>natgridW.c</t>
-  </si>
-  <si>
-    <t>ncl2v5dW.c</t>
-  </si>
-  <si>
-    <t>ncolorW.c</t>
-  </si>
-  <si>
-    <t>nglogoW.c</t>
-  </si>
-  <si>
-    <t>ngmiscW.c</t>
-  </si>
-  <si>
-    <t>nicevalsW.c</t>
-  </si>
-  <si>
-    <t>objanalW.c</t>
-  </si>
-  <si>
-    <t>omcalc_ccmW.c</t>
-  </si>
-  <si>
-    <t>outputgif.c</t>
-  </si>
-  <si>
-    <t>paleoW.c</t>
-  </si>
-  <si>
-    <t>pdfW.c</t>
-  </si>
-  <si>
-    <t>poissonW.c</t>
-  </si>
-  <si>
-    <t>prcwatW.c</t>
-  </si>
-  <si>
-    <t>preshybW.c</t>
-  </si>
-  <si>
-    <t>pressigW.c</t>
-  </si>
-  <si>
-    <t>probtestW.c</t>
-  </si>
-  <si>
-    <t>randomW.c</t>
-  </si>
-  <si>
-    <t>rcmW.c</t>
-  </si>
-  <si>
-    <t>reduce2reg.f90</t>
-  </si>
-  <si>
-    <t>regcoefW.c</t>
-  </si>
-  <si>
-    <t>regridtst.f90</t>
-  </si>
-  <si>
-    <t>relhumW.c</t>
-  </si>
-  <si>
-    <t>remapW.c</t>
-  </si>
-  <si>
-    <t>rhombtriW.c</t>
-  </si>
-  <si>
-    <t>ripW.c</t>
   </si>
 </sst>
 </file>
@@ -573,13 +577,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -911,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A61" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68:C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -922,767 +927,899 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>62</v>
+        <v>91</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>24</v>
+        <v>52</v>
+      </c>
+      <c r="D5" s="6">
+        <v>38946</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="4" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="4" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="4" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="4" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="4" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="4" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="4" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="4" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="4" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="4" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="4" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="4" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="4" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="4" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="4" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="4" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="4" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="4" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="4" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="4" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="4" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="4" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="4" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="4" t="s">
-        <v>97</v>
+        <v>126</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="4" t="s">
-        <v>98</v>
+        <v>127</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="4" t="s">
-        <v>99</v>
+        <v>128</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="4" t="s">
-        <v>100</v>
+        <v>129</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="4" t="s">
-        <v>101</v>
+        <v>130</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="4" t="s">
-        <v>102</v>
+        <v>131</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="4" t="s">
-        <v>103</v>
+        <v>132</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="4" t="s">
-        <v>104</v>
+        <v>133</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
+        <v>134</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
+        <v>135</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
+        <v>136</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
+        <v>137</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
+        <v>138</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
+        <v>139</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
+        <v>0</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
+        <v>1</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
+        <v>2</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
+        <v>4</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
+        <v>5</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
+        <v>6</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
+        <v>7</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
+        <v>8</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
+        <v>9</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
+        <v>10</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
+        <v>11</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
+        <v>12</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
+        <v>13</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
+        <v>15</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
+        <v>16</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
+        <v>17</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="A72" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
+        <v>18</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
+        <v>19</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
+        <v>20</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
+        <v>21</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
+        <v>22</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
+        <v>23</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
+        <v>24</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
+        <v>25</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1">
+        <v>26</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="A81" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
+        <v>27</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
       <c r="A83" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
       <c r="A89" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
       <c r="A90" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
       <c r="A91" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
       <c r="A92" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
       <c r="A93" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
       <c r="A94" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
       <c r="A95" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
       <c r="A96" s="4" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="4" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="4" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="4" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="4" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="4" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="4" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="4" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="4" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="4" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" s="4" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="4" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" s="4" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="4" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="4" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="4" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" s="4" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="4" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="4" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="4" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="4" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="4" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="4" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="4" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="D125" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="4" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" s="4" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" s="4" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
     </row>
     <row r="131" spans="1:1">
@@ -2068,7 +2205,7 @@
     </row>
     <row r="1048576" spans="3:3">
       <c r="C1048576" s="5" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wei'll do all nfp directory
git-svn-id: https://subversion.ucar.edu/ncldev/ncarg/branches/NCL_6_0_0@11719 10fe2890-8a40-4696-8b1d-7ccbb19c398e
</commit_message>
<xml_diff>
--- a/ni/src/lib/nfp/NfpSrcList.xlsx
+++ b/ni/src/lib/nfp/NfpSrcList.xlsx
@@ -19,7 +19,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="142">
+  <si>
+    <t>drwvctc.c</t>
+  </si>
+  <si>
+    <t>dsgridW.c</t>
+  </si>
+  <si>
+    <t>dtrendW.c</t>
+  </si>
+  <si>
+    <t>dzheightW.c</t>
+  </si>
+  <si>
+    <t>echoW.c</t>
+  </si>
+  <si>
+    <t>eofW.c</t>
+  </si>
+  <si>
+    <t>erfW.c</t>
+  </si>
+  <si>
+    <t>extaperW.c</t>
+  </si>
+  <si>
+    <t>ezfftW.c</t>
+  </si>
+  <si>
+    <t>fft2dW.c</t>
+  </si>
+  <si>
+    <t>filterxW.c</t>
+  </si>
+  <si>
+    <t>finitediffW.c</t>
+  </si>
+  <si>
+    <t>fitgridW.c</t>
+  </si>
+  <si>
+    <t>fluxEddyW.c</t>
+  </si>
+  <si>
+    <t>fourinfoW.c</t>
+  </si>
+  <si>
+    <t>gausW.c</t>
+  </si>
+  <si>
+    <t>gtripleW.c</t>
+  </si>
+  <si>
+    <t>hydroW.c</t>
+  </si>
+  <si>
+    <t>hyi2hyoW.c</t>
+  </si>
+  <si>
+    <t>indW.c</t>
+  </si>
+  <si>
+    <t>int2pW.c</t>
+  </si>
+  <si>
+    <t>invmatrixW.c</t>
+  </si>
+  <si>
+    <t>julGregW.c</t>
+  </si>
+  <si>
+    <t>kronprodW.c</t>
+  </si>
+  <si>
+    <t>linint2W.c</t>
+  </si>
+  <si>
+    <t>linmsgW.c</t>
+  </si>
+  <si>
+    <t>linroodW.c</t>
+  </si>
+  <si>
+    <t>locminmaxW.c</t>
+  </si>
+  <si>
+    <t>lspolyW.c</t>
+  </si>
+  <si>
+    <t>Wei</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Updated</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>mapgciW.c</t>
   </si>
@@ -411,93 +506,6 @@
   </si>
   <si>
     <t>dimavgwgtW.c</t>
-  </si>
-  <si>
-    <t>drwvctc.c</t>
-  </si>
-  <si>
-    <t>dsgridW.c</t>
-  </si>
-  <si>
-    <t>dtrendW.c</t>
-  </si>
-  <si>
-    <t>dzheightW.c</t>
-  </si>
-  <si>
-    <t>echoW.c</t>
-  </si>
-  <si>
-    <t>eofW.c</t>
-  </si>
-  <si>
-    <t>erfW.c</t>
-  </si>
-  <si>
-    <t>extaperW.c</t>
-  </si>
-  <si>
-    <t>ezfftW.c</t>
-  </si>
-  <si>
-    <t>fft2dW.c</t>
-  </si>
-  <si>
-    <t>filterxW.c</t>
-  </si>
-  <si>
-    <t>finitediffW.c</t>
-  </si>
-  <si>
-    <t>fitgridW.c</t>
-  </si>
-  <si>
-    <t>fluxEddyW.c</t>
-  </si>
-  <si>
-    <t>fourinfoW.c</t>
-  </si>
-  <si>
-    <t>gausW.c</t>
-  </si>
-  <si>
-    <t>gtripleW.c</t>
-  </si>
-  <si>
-    <t>hydroW.c</t>
-  </si>
-  <si>
-    <t>hyi2hyoW.c</t>
-  </si>
-  <si>
-    <t>indW.c</t>
-  </si>
-  <si>
-    <t>int2pW.c</t>
-  </si>
-  <si>
-    <t>invmatrixW.c</t>
-  </si>
-  <si>
-    <t>julGregW.c</t>
-  </si>
-  <si>
-    <t>kronprodW.c</t>
-  </si>
-  <si>
-    <t>linint2W.c</t>
-  </si>
-  <si>
-    <t>linmsgW.c</t>
-  </si>
-  <si>
-    <t>linroodW.c</t>
-  </si>
-  <si>
-    <t>locminmaxW.c</t>
-  </si>
-  <si>
-    <t>lspolyW.c</t>
   </si>
 </sst>
 </file>
@@ -916,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A61" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68:C81"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -927,40 +935,40 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>119</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="D5" s="6">
         <v>38946</v>
@@ -968,900 +976,1090 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>53</v>
+        <v>84</v>
+      </c>
+      <c r="D6" s="6">
+        <v>38946</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
+      </c>
+      <c r="D8" s="6">
+        <v>38946</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
+      </c>
+      <c r="D9" s="6">
+        <v>38946</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
+      </c>
+      <c r="D10" s="6">
+        <v>38946</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
+      </c>
+      <c r="D11" s="6">
+        <v>38946</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
+      </c>
+      <c r="D13" s="6">
+        <v>38946</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
+      </c>
+      <c r="D14" s="6">
+        <v>38946</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>101</v>
+        <v>132</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
+      </c>
+      <c r="D15" s="6">
+        <v>38951</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="4" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>86</v>
+      </c>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="4" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="4" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>81</v>
+      </c>
+      <c r="D19" s="6">
+        <v>38951</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>81</v>
+      </c>
+      <c r="D20" s="6">
+        <v>38951</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="4" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>81</v>
+      </c>
+      <c r="D21" s="6">
+        <v>38951</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="4" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>81</v>
+      </c>
+      <c r="D22" s="6">
+        <v>38951</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>81</v>
+      </c>
+      <c r="D23" s="6">
+        <v>38951</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
-        <v>111</v>
+        <v>0</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>81</v>
+      </c>
+      <c r="D26" s="6">
+        <v>38951</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="4" t="s">
-        <v>113</v>
+        <v>2</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>81</v>
+      </c>
+      <c r="D27" s="6">
+        <v>38951</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>114</v>
+        <v>3</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
-        <v>115</v>
+        <v>4</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
-        <v>116</v>
+        <v>5</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
-        <v>117</v>
+        <v>6</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
-        <v>118</v>
+        <v>7</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="4" t="s">
-        <v>119</v>
+        <v>8</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="4" t="s">
-        <v>120</v>
+        <v>9</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4" t="s">
-        <v>121</v>
+        <v>10</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="4" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="4" t="s">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="4" t="s">
-        <v>124</v>
+        <v>13</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="4" t="s">
-        <v>125</v>
+        <v>14</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="4" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="4" t="s">
-        <v>127</v>
+        <v>16</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="4" t="s">
-        <v>128</v>
+        <v>17</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="4" t="s">
-        <v>129</v>
+        <v>18</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="4" t="s">
-        <v>130</v>
+        <v>19</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="4" t="s">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="4" t="s">
-        <v>132</v>
+        <v>21</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="4" t="s">
-        <v>133</v>
+        <v>22</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="4" t="s">
-        <v>134</v>
+        <v>23</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="4" t="s">
-        <v>135</v>
+        <v>24</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="4" t="s">
-        <v>136</v>
+        <v>25</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="4" t="s">
-        <v>137</v>
+        <v>26</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="4" t="s">
-        <v>138</v>
+        <v>27</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="4" t="s">
-        <v>139</v>
+        <v>28</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="4" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="4" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="4" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="4" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="4" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="4" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="4" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="4" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="4" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="4" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="4" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="4" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="4" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="4" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="4" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="4" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="4" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="4" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="4" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="4" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="4" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="4" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="4" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="4" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="4" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="4" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="4" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="4" t="s">
-        <v>28</v>
+        <v>59</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="4" t="s">
-        <v>29</v>
+        <v>60</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="4" t="s">
-        <v>30</v>
+        <v>61</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="4" t="s">
-        <v>31</v>
+        <v>62</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="4" t="s">
-        <v>32</v>
+        <v>63</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="4" t="s">
-        <v>33</v>
+        <v>64</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="4" t="s">
-        <v>34</v>
+        <v>65</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="4" t="s">
-        <v>35</v>
+        <v>66</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="4" t="s">
-        <v>36</v>
+        <v>67</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="4" t="s">
-        <v>37</v>
+        <v>68</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="4" t="s">
-        <v>38</v>
+        <v>69</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="4" t="s">
-        <v>39</v>
+        <v>70</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="4" t="s">
-        <v>40</v>
+        <v>71</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="4" t="s">
-        <v>41</v>
+        <v>72</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1">
+        <v>73</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1">
+        <v>74</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1">
+        <v>75</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
+        <v>76</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1">
+        <v>77</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
+        <v>78</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
+        <v>79</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
+        <v>80</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
+        <v>88</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1">
+        <v>89</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1">
+        <v>90</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1">
+        <v>91</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
       <c r="A108" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1">
+        <v>92</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
       <c r="A109" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1">
+        <v>93</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1">
+        <v>94</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
       <c r="A111" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1">
+        <v>95</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
       <c r="A112" s="4" t="s">
-        <v>65</v>
+        <v>96</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="4" t="s">
-        <v>66</v>
+        <v>97</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
-        <v>67</v>
+        <v>98</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="4" t="s">
-        <v>68</v>
+        <v>99</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="4" t="s">
-        <v>69</v>
+        <v>100</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
-        <v>74</v>
+        <v>105</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="4" t="s">
-        <v>75</v>
+        <v>106</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="4" t="s">
-        <v>76</v>
+        <v>107</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="4" t="s">
-        <v>77</v>
+        <v>108</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="4" t="s">
-        <v>78</v>
+        <v>109</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="4" t="s">
-        <v>79</v>
+        <v>110</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
-        <v>80</v>
+        <v>111</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="D125" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
-        <v>83</v>
+        <v>114</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="4" t="s">
-        <v>84</v>
+        <v>115</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1">
+        <v>116</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
       <c r="A129" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1">
+        <v>117</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
       <c r="A130" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1">
+        <v>118</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
       <c r="A131" s="4"/>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:3">
       <c r="A132" s="4"/>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:3">
       <c r="A133" s="4"/>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:3">
       <c r="A134" s="4"/>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:3">
       <c r="A135" s="4"/>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:3">
       <c r="A136" s="4"/>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:3">
       <c r="A137" s="4"/>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:3">
       <c r="A138" s="4"/>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:3">
       <c r="A139" s="4"/>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:3">
       <c r="A140" s="4"/>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:3">
       <c r="A141" s="4"/>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:3">
       <c r="A142" s="4"/>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:3">
       <c r="A143" s="4"/>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:3">
       <c r="A144" s="4"/>
     </row>
     <row r="145" spans="1:1">
@@ -2205,7 +2403,7 @@
     </row>
     <row r="1048576" spans="3:3">
       <c r="C1048576" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>